<commit_message>
HP: ExcelToStringArray extended with write methods
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Zipfiles" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>item2</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Student Submits</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Results</t>
   </si>
 </sst>
 </file>
@@ -90,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,13 +122,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,12 +558,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
HP: Logger added. ExcelMng updated
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Zipfiles" sheetId="1" r:id="rId1"/>
+    <sheet name="ZipFiles" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
HP: Writing check results to students.xlsx. TOIMII
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ZipFiles" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>item2</t>
   </si>
@@ -76,6 +76,37 @@
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Testcase1</t>
+  </si>
+  <si>
+    <t>Testcase2</t>
+  </si>
+  <si>
+    <t>Testcase3</t>
+  </si>
+  <si>
+    <t>Testcase4</t>
+  </si>
+  <si>
+    <t>SUBMIT(1) TESTCASE(1) RESULT MSG:(TESTCASE#1:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>SUBMIT(2) TESTCASE(1) RESULT MSG:(TESTCASE#1:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>SUBMIT(3) TESTCASE(1) RESULT MSG:(TESTCASE#1:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>SUBMIT(4) TESTCASE(1) RESULT MSG:(TESTCASE#1:EQUAL
+)</t>
   </si>
 </sst>
 </file>
@@ -135,10 +166,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,15 +476,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -558,20 +592,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G10"/>
+  <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="75.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -584,12 +628,43 @@
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP: Operation error message propagation.
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>item2</t>
   </si>
@@ -105,12 +105,30 @@
 )</t>
   </si>
   <si>
-    <t>SUBMIT(4) TESTCASE(1) RESULT MSG:(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
     <t>SUBMIT(4) TESTCASE(1) RESULT MSG:(TESTCASE#1:NOT_EQUAL
 )</t>
+  </si>
+  <si>
+    <t>SUBMIT(4) TESTCASE(1) OPER ERRORS:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(1) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(2) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(3) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(4) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(1) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
   </si>
 </sst>
 </file>
@@ -654,22 +672,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP: Testing 2 testcases
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>item2</t>
   </si>
@@ -91,25 +91,6 @@
   </si>
   <si>
     <t>Testcase4</t>
-  </si>
-  <si>
-    <t>SUBMIT(1) TESTCASE(1) RESULT MSG:(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>SUBMIT(2) TESTCASE(1) RESULT MSG:(TESTCASE#1:NOT_EQUAL
-)</t>
-  </si>
-  <si>
-    <t>SUBMIT(3) TESTCASE(1) RESULT MSG:(TESTCASE#1:NOT_EQUAL
-)</t>
-  </si>
-  <si>
-    <t>SUBMIT(4) TESTCASE(1) RESULT MSG:(TESTCASE#1:NOT_EQUAL
-)</t>
-  </si>
-  <si>
-    <t>SUBMIT(4) TESTCASE(1) OPER ERRORS:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
   </si>
   <si>
     <t>RESULT: SUBMIT(1) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
@@ -128,7 +109,38 @@
 )</t>
   </si>
   <si>
+    <t>RESULT: SUBMIT(1) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(2) TESTCASE(2) MSG:(TESTCASE#2:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(3) TESTCASE(2) MSG:(TESTCASE#2:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(4) TESTCASE(2) MSG:(TESTCASE#2:NOT_EQUAL
+)</t>
+  </si>
+  <si>
+    <t>Errors TC1</t>
+  </si>
+  <si>
+    <t>Errors TC2</t>
+  </si>
+  <si>
+    <t>Errors TC3</t>
+  </si>
+  <si>
+    <t>Errors TC4</t>
+  </si>
+  <si>
     <t>ERROR: SUBMIT(4) TESTCASE(1) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
   </si>
 </sst>
 </file>
@@ -615,30 +627,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A2:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="75.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -669,28 +687,56 @@
       <c r="J10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G12" s="3" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G13" s="3" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" t="s">
-        <v>34</v>
+      <c r="N14" t="s">
+        <v>37</v>
+      </c>
+      <c r="O14" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WPC: new testcases3.xsd and genereted jaxb classes
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>item2</t>
   </si>
@@ -732,6 +732,12 @@
       <c r="H14" t="s">
         <v>32</v>
       </c>
+      <c r="L14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
       <c r="N14" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
HP: XSLTransform with parameter-value lists. TOIMII
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>item2</t>
   </si>
@@ -113,28 +113,28 @@
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(2) MSG:(TESTCASE#2:NOT_EQUAL
+    <t>Errors TC1</t>
+  </si>
+  <si>
+    <t>Errors TC2</t>
+  </si>
+  <si>
+    <t>Errors TC3</t>
+  </si>
+  <si>
+    <t>Errors TC4</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(2) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(2) MSG:(TESTCASE#2:NOT_EQUAL
+    <t>RESULT: SUBMIT(3) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(4) TESTCASE(2) MSG:(TESTCASE#2:NOT_EQUAL
+    <t>RESULT: SUBMIT(4) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
 )</t>
-  </si>
-  <si>
-    <t>Errors TC1</t>
-  </si>
-  <si>
-    <t>Errors TC2</t>
-  </si>
-  <si>
-    <t>Errors TC3</t>
-  </si>
-  <si>
-    <t>Errors TC4</t>
   </si>
   <si>
     <t>ERROR: SUBMIT(4) TESTCASE(1) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
@@ -147,7 +147,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,12 +200,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,9 +519,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -629,21 +631,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="3" max="3" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="25.21875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -689,16 +691,16 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -714,7 +716,7 @@
         <v>26</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -722,26 +724,20 @@
         <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M14" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" t="s">
-        <v>37</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="M14" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HP: XMLValidationCheck class added
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>item2</t>
   </si>
@@ -93,70 +93,70 @@
     <t>Testcase4</t>
   </si>
   <si>
+    <t>Errors TC1</t>
+  </si>
+  <si>
+    <t>Errors TC2</t>
+  </si>
+  <si>
+    <t>Errors TC3</t>
+  </si>
+  <si>
+    <t>Errors TC4</t>
+  </si>
+  <si>
     <t>RESULT: SUBMIT(1) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
 )</t>
   </si>
   <si>
+    <t>RESULT: SUBMIT(1) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(1) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+)</t>
+  </si>
+  <si>
     <t>RESULT: SUBMIT(2) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
 )</t>
   </si>
   <si>
+    <t>RESULT: SUBMIT(2) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(2) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+)</t>
+  </si>
+  <si>
     <t>RESULT: SUBMIT(3) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
 )</t>
   </si>
   <si>
+    <t>RESULT: SUBMIT(3) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(3) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+)</t>
+  </si>
+  <si>
     <t>RESULT: SUBMIT(4) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(1) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>Errors TC1</t>
-  </si>
-  <si>
-    <t>Errors TC2</t>
-  </si>
-  <si>
-    <t>Errors TC3</t>
-  </si>
-  <si>
-    <t>Errors TC4</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
     <t>RESULT: SUBMIT(4) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
+    <t>RESULT: SUBMIT(4) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+)</t>
+  </si>
+  <si>
     <t>ERROR: SUBMIT(4) TESTCASE(1) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
   </si>
   <si>
     <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(1) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(4) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
-)</t>
   </si>
 </sst>
 </file>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +660,8 @@
     <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" width="25.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="25.21875" collapsed="true"/>
     <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -707,70 +708,68 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" t="s">
         <v>34</v>
-      </c>
-      <c r="I12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="N14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HP: Init Processing added
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ZipFiles" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="MainInfo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>item2</t>
   </si>
@@ -157,6 +157,30 @@
   </si>
   <si>
     <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
+  </si>
+  <si>
+    <t>MainInfo</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U1E1_1_sub2.xml</t>
+  </si>
+  <si>
+    <t>TaskFlowXmlFile</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ZipFilesSheet</t>
+  </si>
+  <si>
+    <t>ZipFiles</t>
+  </si>
+  <si>
+    <t>ResultsSheet</t>
   </si>
 </sst>
 </file>
@@ -648,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -778,12 +802,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HP: Excel Management updated for new sub round
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="ZipFiles" sheetId="1" r:id="rId1"/>
-    <sheet name="Results" sheetId="2" r:id="rId2"/>
-    <sheet name="MainInfo" sheetId="3" r:id="rId3"/>
+    <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
+    <sheet name="ZipFiles" sheetId="1" r:id="rId2"/>
+    <sheet name="Results" sheetId="2" r:id="rId3"/>
+    <sheet name="ZipFiles_U1_sub3" sheetId="4" r:id="rId4"/>
+    <sheet name="Results_U1_sub3" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>item2</t>
   </si>
@@ -105,6 +107,45 @@
     <t>Errors TC4</t>
   </si>
   <si>
+    <t>MainInfo</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U1E1_1_sub2.xml</t>
+  </si>
+  <si>
+    <t>TaskFlowXmlFile</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ZipFilesSheet</t>
+  </si>
+  <si>
+    <t>ZipFiles</t>
+  </si>
+  <si>
+    <t>ResultsSheet</t>
+  </si>
+  <si>
+    <t>ZipFileCount</t>
+  </si>
+  <si>
+    <t>StudentZipFileFolder</t>
+  </si>
+  <si>
+    <t>ReferenceZipFileFolder</t>
+  </si>
+  <si>
+    <t>ReferenceZipFile</t>
+  </si>
+  <si>
+    <t>RoundU1_sub2_reference.zip</t>
+  </si>
+  <si>
     <t>RESULT: SUBMIT(1) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
 )</t>
   </si>
@@ -159,35 +200,31 @@
     <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
   </si>
   <si>
-    <t>MainInfo</t>
-  </si>
-  <si>
-    <t>data/taskflow/taskflow3_U1E1_1_sub2.xml</t>
-  </si>
-  <si>
-    <t>TaskFlowXmlFile</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>ZipFilesSheet</t>
-  </si>
-  <si>
-    <t>ZipFiles</t>
-  </si>
-  <si>
-    <t>ResultsSheet</t>
+    <t>data/zips/RoundU1_sub2/</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U1E1_2_sub3.xml</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1_sub3</t>
+  </si>
+  <si>
+    <t>Results_U1_sub3</t>
+  </si>
+  <si>
+    <t>data/zips/RoundU1_sub3/</t>
+  </si>
+  <si>
+    <t>RoundU1_sub3_reference.zip</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -250,6 +287,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,17 +595,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f>TEXT(ZipFiles!E9,"0")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="6" t="str">
+        <f>TEXT(ZipFiles!E19,"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -578,6 +779,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="5">
+        <f>COUNTA(E11:E100)</f>
+        <v>4</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
@@ -662,138 +874,6 @@
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O14"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="25.21875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="G14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -802,56 +882,157 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A2:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="3" max="3" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="29" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.21875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="I12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="H13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="I13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HP: Testing Validation operation.
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
   <si>
     <t>item2</t>
   </si>
@@ -219,12 +219,76 @@
   </si>
   <si>
     <t>TODO</t>
+  </si>
+  <si>
+    <t>Submission: sub3</t>
+  </si>
+  <si>
+    <t>RoundU1_sub3_100000.zip</t>
+  </si>
+  <si>
+    <t>RoundU1_sub3_100001.zip</t>
+  </si>
+  <si>
+    <t>RoundU1_sub3_100002.zip</t>
+  </si>
+  <si>
+    <t>RoundU1_sub3_100003.zip</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(1) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(2) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(3) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
+  </si>
+  <si>
+    <t>RESULT: SUBMIT(4) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(1) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(1) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,14 +661,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -706,8 +770,8 @@
         <v>37</v>
       </c>
       <c r="C23" s="6" t="str">
-        <f>TEXT(ZipFiles!E19,"0")</f>
-        <v>0</v>
+        <f>TEXT(ZipFiles_U1_sub3!E9,"0")</f>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>62</v>
@@ -756,14 +820,14 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -885,20 +949,20 @@
   <dimension ref="A2:O14"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:AC18"/>
+      <selection activeCell="A9" sqref="A9:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="29" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.21875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="25.21875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -1015,24 +1079,253 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="29.88671875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="5">
+        <f>COUNTA(E11:E100)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100001</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>100002</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>100003</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A9:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" t="s">
+        <v>82</v>
+      </c>
+      <c r="M14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HP: Taskflow can now be selected in student.xlsx
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -8,17 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
-    <sheet name="ZipFiles" sheetId="1" r:id="rId2"/>
-    <sheet name="Results" sheetId="2" r:id="rId3"/>
-    <sheet name="ZipFiles_U1_sub3" sheetId="4" r:id="rId4"/>
-    <sheet name="Results_U1_sub3" sheetId="5" r:id="rId5"/>
+    <sheet name="ZipFiles_U1_sub2" sheetId="1" r:id="rId2"/>
+    <sheet name="Results_U1_sub2" sheetId="2" r:id="rId3"/>
+    <sheet name="ZipFiles_U3_sub1" sheetId="4" r:id="rId4"/>
+    <sheet name="Results_U3_sub1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
   <si>
     <t>item2</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>ZipFilesSheet</t>
-  </si>
-  <si>
-    <t>ZipFiles</t>
   </si>
   <si>
     <t>ResultsSheet</t>
@@ -203,85 +200,71 @@
     <t>data/zips/RoundU1_sub2/</t>
   </si>
   <si>
-    <t>data/taskflow/taskflow3_U1E1_2_sub3.xml</t>
-  </si>
-  <si>
-    <t>ZipFiles_U1_sub3</t>
-  </si>
-  <si>
-    <t>Results_U1_sub3</t>
-  </si>
-  <si>
-    <t>data/zips/RoundU1_sub3/</t>
-  </si>
-  <si>
-    <t>RoundU1_sub3_reference.zip</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Submission: sub3</t>
-  </si>
-  <si>
-    <t>RoundU1_sub3_100000.zip</t>
-  </si>
-  <si>
-    <t>RoundU1_sub3_100001.zip</t>
-  </si>
-  <si>
-    <t>RoundU1_sub3_100002.zip</t>
-  </si>
-  <si>
-    <t>RoundU1_sub3_100003.zip</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(1) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
+    <t>data/taskflow/taskflow3_U3E1_1_sub1.xml</t>
+  </si>
+  <si>
+    <t>ZipFiles_U3_sub1</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Submission:</t>
+  </si>
+  <si>
+    <t>sub1</t>
+  </si>
+  <si>
+    <t>Round_U3_sub1_100000.zip</t>
+  </si>
+  <si>
+    <t>Round_U3_sub1_100001.zip</t>
+  </si>
+  <si>
+    <t>Round_U3_sub1_reference.zip</t>
+  </si>
+  <si>
+    <t>Results_U3_sub1</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1_sub2</t>
+  </si>
+  <si>
+    <t>Results_U1_sub2</t>
+  </si>
+  <si>
+    <t>NOTE: old file name pattern used</t>
+  </si>
+  <si>
+    <t>data/zips/Round_U3_tests/</t>
   </si>
   <si>
     <t>RESULT: SUBMIT(2) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
 )</t>
   </si>
   <si>
-    <t>ERROR: SUBMIT(2) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(3) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(4) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:schema_reference.4: Failed to read schema document 'file:/C:/Users/Pekka%20Aarnio/git/egit_xml_projects/SerialXmlZipProcessor/RoundU1/exU1E1_2/src/Employee.xsd', because 1) could not find the document; 2) the document could not be read; 3) the root element of the document is not &lt;xsd:schema&gt;.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(1) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(2) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(3) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'schema'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(1) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(2) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(3) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.operator.XMLValidationCheck ERROR:cvc-elt.1: Cannot find the declaration of element 'Employee'.)</t>
+    <t>TASKFLOW 1</t>
+  </si>
+  <si>
+    <t>TASKFLOW 2</t>
+  </si>
+  <si>
+    <t>TASKFLOW 3</t>
+  </si>
+  <si>
+    <t>TASKFLOW 4</t>
+  </si>
+  <si>
+    <t>KeyFirstRow</t>
+  </si>
+  <si>
+    <t>KeyLastRow</t>
+  </si>
+  <si>
+    <t>SELECT TASKFLOW Nr:</t>
+  </si>
+  <si>
+    <t>TASKFLOW ROWS</t>
   </si>
 </sst>
 </file>
@@ -298,12 +281,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -342,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -357,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,24 +651,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="str">
+        <f>TEXT($C$2*10,"0")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="str">
+        <f>TEXT($C$2*10 + 8,"0")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -684,7 +724,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -692,56 +732,70 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>34</v>
       </c>
       <c r="C12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f>TEXT(ZipFiles_U1_sub2!E9,"0")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="6" t="str">
-        <f>TEXT(ZipFiles!E9,"0")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
@@ -749,64 +803,87 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="str">
+        <f>TEXT(ZipFiles_U3_sub1!E9,"0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="6" t="str">
-        <f>TEXT(ZipFiles_U1_sub3!E9,"0")</f>
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
       <c r="C26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +922,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1022,53 +1099,53 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
         <v>42</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>43</v>
-      </c>
-      <c r="I11" t="s">
-        <v>44</v>
       </c>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>46</v>
-      </c>
-      <c r="I12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
         <v>48</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>49</v>
-      </c>
-      <c r="I13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
         <v>51</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>52</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -1079,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,23 +1177,26 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E9" s="5">
         <f>COUNTA(E11:E100)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1150,7 +1230,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1167,41 +1247,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1">
-        <v>100002</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1">
-        <v>100003</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1211,13 +1257,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:O10"/>
+  <dimension ref="A9:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.77734375" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
@@ -1269,60 +1319,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11">
-      <c r="G11" t="s">
+    <row r="11" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="G11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" t="s">
-        <v>79</v>
-      </c>
-      <c r="M11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="G12" t="s">
+    </row>
+    <row r="12" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="G13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L13" t="s">
-        <v>81</v>
-      </c>
-      <c r="M13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="G14" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" t="s">
-        <v>82</v>
-      </c>
-      <c r="M14" t="s">
-        <v>82</v>
+      <c r="H12" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP: testcase4.xsd updated. Points added to excel
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
   <si>
     <t>item2</t>
   </si>
@@ -143,135 +143,158 @@
     <t>RoundU1_sub2_reference.zip</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(1) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
+    <t>data/zips/RoundU1_sub2/</t>
+  </si>
+  <si>
+    <t>data/taskflow/taskflow3_U3E1_1_sub1.xml</t>
+  </si>
+  <si>
+    <t>ZipFiles_U3_sub1</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Submission:</t>
+  </si>
+  <si>
+    <t>sub1</t>
+  </si>
+  <si>
+    <t>Round_U3_sub1_100000.zip</t>
+  </si>
+  <si>
+    <t>Round_U3_sub1_100001.zip</t>
+  </si>
+  <si>
+    <t>Round_U3_sub1_reference.zip</t>
+  </si>
+  <si>
+    <t>Results_U3_sub1</t>
+  </si>
+  <si>
+    <t>ZipFiles_U1_sub2</t>
+  </si>
+  <si>
+    <t>Results_U1_sub2</t>
+  </si>
+  <si>
+    <t>NOTE: old file name pattern used</t>
+  </si>
+  <si>
+    <t>data/zips/Round_U3_tests/</t>
+  </si>
+  <si>
+    <t>TASKFLOW 1</t>
+  </si>
+  <si>
+    <t>TASKFLOW 2</t>
+  </si>
+  <si>
+    <t>TASKFLOW 3</t>
+  </si>
+  <si>
+    <t>TASKFLOW 4</t>
+  </si>
+  <si>
+    <t>KeyFirstRow</t>
+  </si>
+  <si>
+    <t>KeyLastRow</t>
+  </si>
+  <si>
+    <t>SELECT TASKFLOW Nr:</t>
+  </si>
+  <si>
+    <t>TASKFLOW ROWS</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(1)  FLOW(true) MSG(TESTCASE#1:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(1) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+    <t>RESULT(1) TCASE(2)  FLOW(true) MSG(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(1) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+    <t>RESULT(1) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
+    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE#1:NOT_EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+    <t>RESULT(2) TCASE(2)  FLOW(true) MSG(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+    <t>RESULT(2) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
+    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE#1:NOT_EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(3) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(4) TESTCASE(1) MSG:(TESTCASE#1:NOT_EQUAL
+    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE#1:NOT_EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(4) TESTCASE(2) MSG:(TESTCASE#2:EQUAL
+    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE#2:EQUAL
 )</t>
   </si>
   <si>
-    <t>RESULT: SUBMIT(4) TESTCASE(3) MSG:(TESTCASE#3:EQUAL
+    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
 )</t>
   </si>
   <si>
+    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE#1:EQUAL
+)</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Points TC1</t>
+  </si>
+  <si>
+    <t>Points TC2</t>
+  </si>
+  <si>
+    <t>Points TC3</t>
+  </si>
+  <si>
+    <t>Points TC4</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>ERROR: SUBMIT(4) TESTCASE(1) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
   </si>
   <si>
     <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
-  </si>
-  <si>
-    <t>data/zips/RoundU1_sub2/</t>
-  </si>
-  <si>
-    <t>data/taskflow/taskflow3_U3E1_1_sub1.xml</t>
-  </si>
-  <si>
-    <t>ZipFiles_U3_sub1</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>Submission:</t>
-  </si>
-  <si>
-    <t>sub1</t>
-  </si>
-  <si>
-    <t>Round_U3_sub1_100000.zip</t>
-  </si>
-  <si>
-    <t>Round_U3_sub1_100001.zip</t>
-  </si>
-  <si>
-    <t>Round_U3_sub1_reference.zip</t>
-  </si>
-  <si>
-    <t>Results_U3_sub1</t>
-  </si>
-  <si>
-    <t>ZipFiles_U1_sub2</t>
-  </si>
-  <si>
-    <t>Results_U1_sub2</t>
-  </si>
-  <si>
-    <t>NOTE: old file name pattern used</t>
-  </si>
-  <si>
-    <t>data/zips/Round_U3_tests/</t>
-  </si>
-  <si>
-    <t>RESULT: SUBMIT(2) TESTCASE(1) MSG:(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>TASKFLOW 1</t>
-  </si>
-  <si>
-    <t>TASKFLOW 2</t>
-  </si>
-  <si>
-    <t>TASKFLOW 3</t>
-  </si>
-  <si>
-    <t>TASKFLOW 4</t>
-  </si>
-  <si>
-    <t>KeyFirstRow</t>
-  </si>
-  <si>
-    <t>KeyLastRow</t>
-  </si>
-  <si>
-    <t>SELECT TASKFLOW Nr:</t>
-  </si>
-  <si>
-    <t>TASKFLOW ROWS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -653,15 +676,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -671,15 +694,15 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,28 +715,28 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C5" t="str">
         <f>TEXT($C$2*10,"0")</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C6" t="str">
         <f>TEXT($C$2*10 + 8,"0")</f>
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,7 +760,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -754,10 +777,10 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -765,10 +788,10 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -779,7 +802,7 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -787,12 +810,12 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -808,7 +831,7 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
@@ -816,7 +839,7 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -833,7 +856,7 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
@@ -841,7 +864,7 @@
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
@@ -849,7 +872,7 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
@@ -857,12 +880,12 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
@@ -875,7 +898,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
@@ -902,9 +925,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1023,36 +1046,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O14"/>
+  <dimension ref="A2:T14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:R10"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:BK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="25.21875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="3" max="3" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.21875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="29" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.21875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1085,69 +1108,115 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="L12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="L13" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" t="s">
+        <v>82</v>
+      </c>
+      <c r="N13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N14" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>84</v>
+      </c>
+      <c r="R14" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,7 +1233,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1177,15 +1246,15 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1230,7 +1299,7 @@
         <v>100000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1247,7 +1316,7 @@
         <v>100001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1257,24 +1326,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:O12"/>
+  <dimension ref="A9:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="L10" sqref="L10:T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1307,32 +1376,56 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>45</v>
+        <v>67</v>
+      </c>
+      <c r="L12" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP: merge flow and text compare oper updated
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
   <si>
     <t>item2</t>
   </si>
@@ -257,10 +257,6 @@
 )</t>
   </si>
   <si>
-    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
@@ -289,12 +285,73 @@
   </si>
   <si>
     <t>ERROR: SUBMIT(4) TESTCASE(2) MSG:(CLASS:siima.app.XSLTransformer ERROR:Syntax error in '/CATALOG/Plant[(Price&gt;'6.60')] and [(Light='Sun')]'.)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE(1):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE(1):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(
+California Poppy+))</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(California Poppy))</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE(1):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE(2):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,15 +733,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -697,7 +754,7 @@
         <v>61</v>
       </c>
       <c r="C2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -719,7 +776,7 @@
       </c>
       <c r="C5" t="str">
         <f>TEXT($C$2*10,"0")</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -728,7 +785,7 @@
       </c>
       <c r="C6" t="str">
         <f>TEXT($C$2*10 + 8,"0")</f>
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -925,9 +982,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1048,21 +1105,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:BK15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="29" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.21875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="25.21875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1108,16 +1165,16 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>25</v>
@@ -1134,88 +1191,94 @@
     </row>
     <row r="11" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N12" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="L13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N13" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="L14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>84</v>
-      </c>
-      <c r="R14" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1296,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="29.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1334,8 +1397,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1376,16 +1439,16 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>25</v>
@@ -1402,30 +1465,30 @@
     </row>
     <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="L11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" t="s">
         <v>76</v>
-      </c>
-      <c r="M11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>76</v>
-      </c>
-      <c r="M12" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP: AppMainController class added
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="ZipFiles_U3_sub1" sheetId="4" r:id="rId4"/>
     <sheet name="Results_U3_sub1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="89">
   <si>
     <t>item2</t>
   </si>
@@ -207,54 +207,6 @@
   </si>
   <si>
     <t>TASKFLOW ROWS</t>
-  </si>
-  <si>
-    <t>RESULT(1) TCASE(1)  FLOW(true) MSG(TESTCASE#1:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(1) TCASE(2)  FLOW(true) MSG(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(1) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(2) TCASE(1)  FLOW(true) MSG(TESTCASE#1:NOT_EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(2) TCASE(2)  FLOW(true) MSG(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(2) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE#1:NOT_EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE#1:NOT_EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE#2:EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE#3:EQUAL
-)</t>
   </si>
   <si>
     <t>100</t>
@@ -312,39 +264,43 @@
   </si>
   <si>
     <t>RESULT(2) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(2) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(
+California Poppy_x000D_))</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(California Poppy))</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE(1):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE(2):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
 )</t>
   </si>
   <si>
     <t>ERROR: SUBMIT(2) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(
 California Poppy ))</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):NOT-EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(3) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(California Poppy))</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE(1):NOT-COMPARED
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE(2):NOT-COMPARED
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
-)</t>
   </si>
 </sst>
 </file>
@@ -440,6 +396,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -487,7 +446,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,7 +481,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,23 +692,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>61</v>
       </c>
@@ -757,12 +716,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
@@ -770,7 +729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>59</v>
       </c>
@@ -779,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>60</v>
       </c>
@@ -788,7 +747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -796,7 +755,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -804,7 +763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -812,7 +771,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -820,7 +779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -829,7 +788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -840,7 +799,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -851,7 +810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -862,7 +821,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -870,12 +829,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
@@ -883,7 +842,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>31</v>
       </c>
@@ -891,7 +850,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -899,7 +858,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>36</v>
       </c>
@@ -908,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>37</v>
       </c>
@@ -916,7 +875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -924,7 +883,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>39</v>
       </c>
@@ -932,7 +891,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -940,12 +899,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
@@ -953,12 +912,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>32</v>
       </c>
@@ -980,19 +939,19 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1000,18 +959,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="5">
         <f>COUNTA(E11:E100)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1045,7 +1004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1062,7 +1021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1079,7 +1038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1105,34 +1064,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="60.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="68.21875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="58.109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="25.21875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="68.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1165,16 +1126,16 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>25</v>
@@ -1189,96 +1150,96 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H14" t="s">
         <v>86</v>
       </c>
-      <c r="I11" t="s">
-        <v>89</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" t="s">
-        <v>91</v>
-      </c>
-      <c r="L12" t="s">
-        <v>76</v>
-      </c>
-      <c r="M12" t="s">
-        <v>81</v>
-      </c>
-      <c r="N12" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" t="s">
-        <v>95</v>
-      </c>
-      <c r="L13" t="s">
-        <v>76</v>
-      </c>
-      <c r="M13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N13" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="G14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" t="s">
-        <v>98</v>
-      </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>83</v>
-      </c>
-      <c r="R14" t="s">
-        <v>84</v>
+        <v>63</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1294,17 +1255,17 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1312,7 +1273,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1320,18 +1281,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="5">
         <f>COUNTA(E11:E100)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1348,7 +1309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1365,7 +1326,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1395,18 +1356,18 @@
       <selection activeCell="L10" sqref="L10:T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1439,16 +1400,16 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>25</v>
@@ -1463,32 +1424,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M11" t="s">
+      <c r="H12" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="G12" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="L12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="M12" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP: TxtFileReadOper class added
</commit_message>
<xml_diff>
--- a/SerialXmlZipProcessor/data/excel/students.xlsx
+++ b/SerialXmlZipProcessor/data/excel/students.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
   <si>
     <t>item2</t>
   </si>
@@ -264,6 +264,44 @@
   </si>
   <si>
     <t>RESULT(2) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(California Poppy))</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE(1):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE(2):NOT-COMPARED
+)</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>RESULT(1) TCASE(4)  FLOW(true) MSG(TESTCASE(4):EQUAL
+)</t>
+  </si>
+  <si>
+    <t>555</t>
+  </si>
+  <si>
+    <t>RESULT(2) TCASE(4)  FLOW(true) MSG(TESTCASE(4):NOT-EQUAL
 )</t>
   </si>
   <si>
@@ -271,43 +309,27 @@
 California Poppy_x000D_))</t>
   </si>
   <si>
-    <t>RESULT(3) TCASE(1)  FLOW(true) MSG(TESTCASE(1):NOT-EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(2)  FLOW(true) MSG(TESTCASE(2):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>RESULT(3) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(3) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(California Poppy))</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(1)  FLOW(false) MSG(TESTCASE(1):NOT-COMPARED
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(2)  FLOW(false) MSG(TESTCASE(2):NOT-COMPARED
-)</t>
-  </si>
-  <si>
-    <t>RESULT(4) TCASE(3)  FLOW(true) MSG(TESTCASE(3):EQUAL
-)</t>
-  </si>
-  <si>
-    <t>ERROR: SUBMIT(2) TESTCASE(1) MSG:(TEXT COMPARE:DEL:(
-California Poppy-))</t>
+    <t>ERROR: SUBMIT(2) TESTCASE(4) MSG:(TEXT COMPARE:DEL:(6.6))</t>
+  </si>
+  <si>
+    <t>RESULT(3) TCASE(4)  FLOW(true) MSG(TESTCASE(4):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(3) TESTCASE(4) MSG:(TEXT COMPARE:DEL:(Sun))</t>
+  </si>
+  <si>
+    <t>RESULT(4) TCASE(4)  FLOW(true) MSG(TESTCASE(4):NOT-EQUAL
+)</t>
+  </si>
+  <si>
+    <t>ERROR: SUBMIT(4) TESTCASE(4) MSG:(TEXT COMPARE:)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,7 +468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,7 +503,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,19 +718,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>61</v>
       </c>
@@ -716,12 +738,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
@@ -729,7 +751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>59</v>
       </c>
@@ -738,7 +760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>60</v>
       </c>
@@ -747,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -755,7 +777,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -763,7 +785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -771,7 +793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -779,7 +801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -788,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -799,7 +821,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -810,7 +832,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -821,7 +843,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -829,12 +851,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
@@ -842,7 +864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>31</v>
       </c>
@@ -850,7 +872,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -858,7 +880,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>36</v>
       </c>
@@ -867,7 +889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>37</v>
       </c>
@@ -875,7 +897,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -883,7 +905,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>39</v>
       </c>
@@ -891,7 +913,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -899,12 +921,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
@@ -912,12 +934,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>32</v>
       </c>
@@ -939,11 +961,11 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1062,38 +1084,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T14"/>
+  <dimension ref="A2:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="S16" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="60.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="68.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="58.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="60.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="58.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.44140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="26.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="24" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="29.21875" customWidth="1"/>
+    <col min="28" max="28" width="24.109375" customWidth="1"/>
+    <col min="29" max="29" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G11" s="3" t="s">
         <v>73</v>
       </c>
@@ -1160,6 +1185,9 @@
       <c r="I11" t="s">
         <v>77</v>
       </c>
+      <c r="J11" t="s">
+        <v>87</v>
+      </c>
       <c r="L11" s="3" t="s">
         <v>64</v>
       </c>
@@ -1169,8 +1197,24 @@
       <c r="N11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+    </row>
+    <row r="12" spans="1:30" ht="158.4" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
         <v>78</v>
       </c>
@@ -1180,6 +1224,9 @@
       <c r="I12" t="s">
         <v>79</v>
       </c>
+      <c r="J12" t="s">
+        <v>89</v>
+      </c>
       <c r="L12" t="s">
         <v>70</v>
       </c>
@@ -1190,18 +1237,38 @@
         <v>63</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="R12" t="s">
+        <v>69</v>
+      </c>
+      <c r="S12" t="s">
+        <v>63</v>
+      </c>
+      <c r="T12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+    </row>
+    <row r="13" spans="1:30" ht="158.4" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" t="s">
         <v>81</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>82</v>
       </c>
-      <c r="I13" t="s">
-        <v>83</v>
+      <c r="J13" t="s">
+        <v>92</v>
       </c>
       <c r="L13" t="s">
         <v>70</v>
@@ -1213,18 +1280,38 @@
         <v>63</v>
       </c>
       <c r="Q13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="R13" t="s">
+        <v>69</v>
+      </c>
+      <c r="S13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+    </row>
+    <row r="14" spans="1:30" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="G14" s="3" t="s">
+      <c r="H14" t="s">
         <v>85</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>86</v>
       </c>
-      <c r="I14" t="s">
-        <v>87</v>
+      <c r="J14" t="s">
+        <v>94</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>70</v>
@@ -1236,11 +1323,27 @@
         <v>63</v>
       </c>
       <c r="Q14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="S14" t="s">
+        <v>63</v>
+      </c>
+      <c r="T14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="AB14" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="AC14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1255,9 +1358,9 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,18 +1459,18 @@
       <selection activeCell="L10" sqref="L10:T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>